<commit_message>
Adds acceleration calcs to excel sheet.
</commit_message>
<xml_diff>
--- a/Laptime_Simulator_Practice.xlsx
+++ b/Laptime_Simulator_Practice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomwe\Cranfield MSc\GDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomwe\Cranfield MSc\GDP\Laptime-Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A0AABA-AAC3-4522-BCC4-AEB7A2081CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3F9D92-0383-4237-9366-107097DD7481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{428CD39D-5C03-4625-AEA7-BA01D42D1C27}"/>
   </bookViews>
@@ -8379,7 +8379,7 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10685,21 +10685,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="B52:B62"/>
+    <mergeCell ref="A41:A51"/>
+    <mergeCell ref="B41:B51"/>
     <mergeCell ref="B8:B18"/>
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A19:A29"/>
     <mergeCell ref="B19:B29"/>
     <mergeCell ref="B30:B40"/>
     <mergeCell ref="A30:A40"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="B52:B62"/>
-    <mergeCell ref="A41:A51"/>
-    <mergeCell ref="B41:B51"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>